<commit_message>
Commit  Adjective EXERCISES Casus
</commit_message>
<xml_diff>
--- a/data_files/adjectiv.xlsx
+++ b/data_files/adjectiv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python311\django\dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python311\django\dictionary\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4656,8 +4656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
-      <selection activeCell="B330" sqref="B330"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E310" sqref="E310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4666,7 +4666,7 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="74.42578125" customWidth="1"/>
     <col min="6" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="2" customWidth="1"/>
     <col min="9" max="21" width="9.140625" hidden="1" customWidth="1"/>

</xml_diff>